<commit_message>
Added plot of ways to win, numbers aren't reconciled with the blog
</commit_message>
<xml_diff>
--- a/WaystoWin.xlsx
+++ b/WaystoWin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5568FA55-FB94-CE4A-BF92-E09539D3919C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAD6FB0-4E6D-2643-B19B-7EAC1AC5945C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32640" yWindow="-460" windowWidth="28040" windowHeight="17440" xr2:uid="{F363716B-6AFC-E344-83E2-CEB6E89493E8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$144</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -424,10 +424,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62C2E28-F655-AA45-973B-CE432B78AD71}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,7 +488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -740,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>0</v>
       </c>
@@ -1131,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>0</v>
       </c>
@@ -1430,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>0</v>
       </c>
@@ -1476,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>1</v>
       </c>
@@ -1522,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>1</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>1</v>
       </c>
@@ -1706,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>1</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>1</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>1</v>
       </c>
@@ -1913,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>2</v>
       </c>
@@ -2051,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>2</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>2</v>
       </c>
@@ -2258,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>2</v>
       </c>
@@ -2304,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>3</v>
       </c>
@@ -2419,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>3</v>
       </c>
@@ -2534,7 +2535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>3</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>3</v>
       </c>
@@ -2649,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>3</v>
       </c>
@@ -2741,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>3</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>4</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>4</v>
       </c>
@@ -2925,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>4</v>
       </c>
@@ -3040,7 +3041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>4</v>
       </c>
@@ -3178,7 +3179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>5</v>
       </c>
@@ -3247,7 +3248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>5</v>
       </c>
@@ -3385,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>5</v>
       </c>
@@ -3477,7 +3478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>5</v>
       </c>
@@ -3592,7 +3593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>5</v>
       </c>
@@ -3754,6 +3755,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G144" xr:uid="{97D6AD26-2817-3448-AA2C-EB89FCC73C99}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
resource inc/dec works properly now
</commit_message>
<xml_diff>
--- a/WaystoWin.xlsx
+++ b/WaystoWin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/Github Repo/Colonizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAD6FB0-4E6D-2643-B19B-7EAC1AC5945C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4C4A26-1889-9048-B802-E4E1FC4C6A61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32640" yWindow="-460" windowWidth="28040" windowHeight="17440" xr2:uid="{F363716B-6AFC-E344-83E2-CEB6E89493E8}"/>
+    <workbookView xWindow="4640" yWindow="3040" windowWidth="28040" windowHeight="17440" xr2:uid="{F363716B-6AFC-E344-83E2-CEB6E89493E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -424,11 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62C2E28-F655-AA45-973B-CE432B78AD71}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G144"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,7 +487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -741,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>0</v>
       </c>
@@ -1132,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>0</v>
       </c>
@@ -1431,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>0</v>
       </c>
@@ -1477,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>1</v>
       </c>
@@ -1523,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>1</v>
       </c>
@@ -1615,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>1</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>1</v>
       </c>
@@ -1730,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>1</v>
       </c>
@@ -1799,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>1</v>
       </c>
@@ -1914,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>2</v>
       </c>
@@ -2052,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>2</v>
       </c>
@@ -2144,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>2</v>
       </c>
@@ -2259,7 +2258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>2</v>
       </c>
@@ -2305,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>3</v>
       </c>
@@ -2420,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>3</v>
       </c>
@@ -2535,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>3</v>
       </c>
@@ -2627,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>3</v>
       </c>
@@ -2650,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>3</v>
       </c>
@@ -2742,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>3</v>
       </c>
@@ -2765,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>4</v>
       </c>
@@ -2903,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>4</v>
       </c>
@@ -2926,7 +2925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>4</v>
       </c>
@@ -3041,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>4</v>
       </c>
@@ -3179,7 +3178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>5</v>
       </c>
@@ -3248,7 +3247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>5</v>
       </c>
@@ -3386,7 +3385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>5</v>
       </c>
@@ -3478,7 +3477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>5</v>
       </c>
@@ -3593,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>5</v>
       </c>
@@ -3755,13 +3754,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G144" xr:uid="{97D6AD26-2817-3448-AA2C-EB89FCC73C99}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="FALSE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>